<commit_message>
Many initial starbase levels and added ground units to reference
</commit_message>
<xml_diff>
--- a/ReferenceSheet.xlsx
+++ b/ReferenceSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Phoenix Rising Work\EaWXStartingForces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF6A257-C6AA-4AAF-BE4E-CFE439E877CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75250B17-4DC9-4806-A016-DEC9FB46E573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C98BEB51-DB04-4536-A48A-2E267BCF39ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="733">
   <si>
     <t>Name</t>
   </si>
@@ -1614,6 +1614,627 @@
   </si>
   <si>
     <t>Revolt_OldRep_Advanced_Factory</t>
+  </si>
+  <si>
+    <t>SD_6_Droid_Company</t>
+  </si>
+  <si>
+    <t>Storm_Cloud_Car_Company</t>
+  </si>
+  <si>
+    <t>Mandalorian_Soldier_Company</t>
+  </si>
+  <si>
+    <t>Mandalorian_Commando_Company</t>
+  </si>
+  <si>
+    <t>Canderous_Assault_Tank_Company</t>
+  </si>
+  <si>
+    <t>Mandalorian_Soldier_Team</t>
+  </si>
+  <si>
+    <t>Mandalorian_Commando_Team</t>
+  </si>
+  <si>
+    <t>Protocol_Legionnaire_Team</t>
+  </si>
+  <si>
+    <t>Overracer_Speeder_Bike_Company</t>
+  </si>
+  <si>
+    <t>SD_6_Hulk_Infantry_Droid_Company</t>
+  </si>
+  <si>
+    <t>Police_Responder_Team</t>
+  </si>
+  <si>
+    <t>Security_Trooper_Team</t>
+  </si>
+  <si>
+    <t>PDF_Soldier_Team</t>
+  </si>
+  <si>
+    <t>Military_Soldier_Team</t>
+  </si>
+  <si>
+    <t>Scavenger_Team</t>
+  </si>
+  <si>
+    <t>Heavy_Scavenger_Team</t>
+  </si>
+  <si>
+    <t>Light_Mercenary_Team</t>
+  </si>
+  <si>
+    <t>Mercenary_Team</t>
+  </si>
+  <si>
+    <t>Elite_Mercenary_Team</t>
+  </si>
+  <si>
+    <t>Navy_Trooper_Squad</t>
+  </si>
+  <si>
+    <t>Enforcer_Trooper_Squad</t>
+  </si>
+  <si>
+    <t>Army_Guard_Squad</t>
+  </si>
+  <si>
+    <t>Army_Trooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Medium_Armytrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Medic_Armytrooper_Squad</t>
+  </si>
+  <si>
+    <t>Pentastar_Army_Trooper_Squad</t>
+  </si>
+  <si>
+    <t>Pentastar_Medium_Armytrooper_Squad</t>
+  </si>
+  <si>
+    <t>Pentastar_Medic_Armytrooper_Squad</t>
+  </si>
+  <si>
+    <t>EVO_Trooper_Platoon</t>
+  </si>
+  <si>
+    <t>Imperial_Compforce_Assault_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Navy_Commando_Squad</t>
+  </si>
+  <si>
+    <t>Army_Special_Missions_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_ISB_Infiltrator_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_IntSec_Operator_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Medium_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Medic_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Ysalamiri_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Dark_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Shadow_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Royal_Guard_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Elite_Guard_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Nova_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Incinerator_Stormtrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Army_Commando_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Fleet_Commando_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Fleet_Commando_Sniper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Guardian_Protector_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Scout_Trooper_Assault_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Scout_Trooper_Sniper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Scout_Trooper_Commando_Squad</t>
+  </si>
+  <si>
+    <t>Zsinj_Raptor_Squad</t>
+  </si>
+  <si>
+    <t>Zsinj_Raptor_Medic_Squad</t>
+  </si>
+  <si>
+    <t>Storm_Commando_Platoon</t>
+  </si>
+  <si>
+    <t>Imperial_Jumptrooper_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_EWEB_Company</t>
+  </si>
+  <si>
+    <t>Imperial_74Z_Bike_Company</t>
+  </si>
+  <si>
+    <t>Zsinj_74Z_Bike_Company</t>
+  </si>
+  <si>
+    <t>Imperial_BARC_Company</t>
+  </si>
+  <si>
+    <t>Imperial_64Y_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Dwarf_Spider_Droid_Squad</t>
+  </si>
+  <si>
+    <t>Noghri_Assassin_Squad</t>
+  </si>
+  <si>
+    <t>Imperial_Dark_Jedi_Squad</t>
+  </si>
+  <si>
+    <t>Dark_Jedi_Squad</t>
+  </si>
+  <si>
+    <t>Night_Sister_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Chrysalide_Company</t>
+  </si>
+  <si>
+    <t>Imperial_PX10_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_PT_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_RT_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_MP_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_ST_Company</t>
+  </si>
+  <si>
+    <t>Imperial_1L_Tank_Company</t>
+  </si>
+  <si>
+    <t>Imperial_ULAV_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_ST_A_Company</t>
+  </si>
+  <si>
+    <t>Imperial_ISP_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Repulsor_Scout_Company</t>
+  </si>
+  <si>
+    <t>Imperial_RTT_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Gaba18_Group</t>
+  </si>
+  <si>
+    <t>Imperial_INT4_Group</t>
+  </si>
+  <si>
+    <t>Imperial_AT_DP_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Skiff_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Chariot_LAV_Company</t>
+  </si>
+  <si>
+    <t>Imperial_TIE_Mauler_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Light_Artillery_Company</t>
+  </si>
+  <si>
+    <t>Imperial_UT_AA_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_AP_Walker_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_AA_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Heavy_Artillery_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Missile_Artillery_Company</t>
+  </si>
+  <si>
+    <t>Imperial_APC_Company</t>
+  </si>
+  <si>
+    <t>Imperial_TX130_Company</t>
+  </si>
+  <si>
+    <t>Imperial_1M_Tank_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Flashblind_Group</t>
+  </si>
+  <si>
+    <t>Imperial_Century_Tank_Company</t>
+  </si>
+  <si>
+    <t>Imperial_TNT_Company</t>
+  </si>
+  <si>
+    <t>Imperial_2M_Company</t>
+  </si>
+  <si>
+    <t>Imperial_S_1_Firehawke_Company</t>
+  </si>
+  <si>
+    <t>Imperial_SA5_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Deathhawk_Group</t>
+  </si>
+  <si>
+    <t>Imperial_SPMAG_Company</t>
+  </si>
+  <si>
+    <t>Imperial_1H_Tank_Company</t>
+  </si>
+  <si>
+    <t>Imperial_1H_Tank_Company_Green</t>
+  </si>
+  <si>
+    <t>Imperial_SPMAT_Company</t>
+  </si>
+  <si>
+    <t>Imperial_LAAT_Group</t>
+  </si>
+  <si>
+    <t>Imperial_IDT_Group</t>
+  </si>
+  <si>
+    <t>Imperial_MAAT_Group</t>
+  </si>
+  <si>
+    <t>Imperial_Nemesis_Gunship_Group</t>
+  </si>
+  <si>
+    <t>Imperial_B5_Juggernaut_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_TE_Walker_Company</t>
+  </si>
+  <si>
+    <t>Imperial_PX4_Company</t>
+  </si>
+  <si>
+    <t>Imperial_TRMB_Company</t>
+  </si>
+  <si>
+    <t>Imperial_A5_Juggernaut_Company</t>
+  </si>
+  <si>
+    <t>Imperial_A9_Fortress_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_AT_Company</t>
+  </si>
+  <si>
+    <t>Imperial_C10_Siege_Tower_Company</t>
+  </si>
+  <si>
+    <t>Imperial_Lancet_Group</t>
+  </si>
+  <si>
+    <t>Imperial_Heavy_Recovery_Vehicle_Company</t>
+  </si>
+  <si>
+    <t>Imperial_AT_AT_Refit_Company</t>
+  </si>
+  <si>
+    <t>Imperial_XR85_Company</t>
+  </si>
+  <si>
+    <t>Imperial_A6_Juggernaut_Company</t>
+  </si>
+  <si>
+    <t>X34_Technical_Company</t>
+  </si>
+  <si>
+    <t>ULAV_Early_Company</t>
+  </si>
+  <si>
+    <t>Espo_Walker_Early_Squad</t>
+  </si>
+  <si>
+    <t>ISP_Company</t>
+  </si>
+  <si>
+    <t>AAC_1_Company</t>
+  </si>
+  <si>
+    <t>Arrow_23_Company</t>
+  </si>
+  <si>
+    <t>AA70_Company</t>
+  </si>
+  <si>
+    <t>T1A_Company</t>
+  </si>
+  <si>
+    <t>T2A_Company</t>
+  </si>
+  <si>
+    <t>Freerunner_Early_Company</t>
+  </si>
+  <si>
+    <t>Freerunner_Assault_Company</t>
+  </si>
+  <si>
+    <t>Freerunner_AA_Company</t>
+  </si>
+  <si>
+    <t>SA5_Company_Early_Company</t>
+  </si>
+  <si>
+    <t>T3A_Company</t>
+  </si>
+  <si>
+    <t>T4A_Company</t>
+  </si>
+  <si>
+    <t>MZ8_Tank_Company</t>
+  </si>
+  <si>
+    <t>A4_Juggernaut_Company</t>
+  </si>
+  <si>
+    <t>Aratech_Battle_Platform_Company</t>
+  </si>
+  <si>
+    <t>Skyhopper_Group</t>
+  </si>
+  <si>
+    <t>Skyhopper_Antivehicle_Group</t>
+  </si>
+  <si>
+    <t>Skyhopper_Primitive_Group</t>
+  </si>
+  <si>
+    <t>Skyhopper_Security_Group</t>
+  </si>
+  <si>
+    <t>Storm_Cloud_Car_Group</t>
+  </si>
+  <si>
+    <t>JX30_Group</t>
+  </si>
+  <si>
+    <t>Rebel_Infantry_Squad</t>
+  </si>
+  <si>
+    <t>Rebel_Infantry_Squad_Deployed</t>
+  </si>
+  <si>
+    <t>Rebel_Support_Infantry_Squad</t>
+  </si>
+  <si>
+    <t>Defense_Trooper_Squad</t>
+  </si>
+  <si>
+    <t>Rebel_Marine_Squad</t>
+  </si>
+  <si>
+    <t>Rebel_Infiltrator_Team</t>
+  </si>
+  <si>
+    <t>Jedi_Squad</t>
+  </si>
+  <si>
+    <t>Rebel_AAC_2_Company</t>
+  </si>
+  <si>
+    <t>Rebel_T1B_Company</t>
+  </si>
+  <si>
+    <t>Rebel_AA5_Company</t>
+  </si>
+  <si>
+    <t>Rebel_Snowspeeder_Wing</t>
+  </si>
+  <si>
+    <t>Rebel_T2B_Company</t>
+  </si>
+  <si>
+    <t>Rebel_Tracker_Company</t>
+  </si>
+  <si>
+    <t>Rebel_MPTL_Company</t>
+  </si>
+  <si>
+    <t>Rebel_Vwing_Group</t>
+  </si>
+  <si>
+    <t>Rebel_T3B_Company</t>
+  </si>
+  <si>
+    <t>Rebel_Gallofree_HTT_Company</t>
+  </si>
+  <si>
+    <t>Rebel_Freerunner_Company</t>
+  </si>
+  <si>
+    <t>Rebel_T4B_Company</t>
+  </si>
+  <si>
+    <t>MAS_2xB_Company</t>
+  </si>
+  <si>
+    <t>Phalanx_Commando_Team</t>
+  </si>
+  <si>
+    <t>Phalanx_Trooper_Squad</t>
+  </si>
+  <si>
+    <t>Phalanx_Medic_Squad</t>
+  </si>
+  <si>
+    <t>Ysalamiri_Phalanx_Squad</t>
+  </si>
+  <si>
+    <t>EotH_Scout_Brigade</t>
+  </si>
+  <si>
+    <t>EotH_Kirov_Brigade</t>
+  </si>
+  <si>
+    <t>Flame_Tank_Company</t>
+  </si>
+  <si>
+    <t>AirStraeker_Company</t>
+  </si>
+  <si>
+    <t>RFT_Brigade</t>
+  </si>
+  <si>
+    <t>MMT_Brigade</t>
+  </si>
+  <si>
+    <t>Mortar_Company</t>
+  </si>
+  <si>
+    <t>Gilzean_Brigade</t>
+  </si>
+  <si>
+    <t>CSA_B1_Droid_Squad</t>
+  </si>
+  <si>
+    <t>CSA_Medium_Droid_Squad</t>
+  </si>
+  <si>
+    <t>Espo_Squad</t>
+  </si>
+  <si>
+    <t>CSA_Medium_Espo_Squad</t>
+  </si>
+  <si>
+    <t>CSA_Medic_Espo_Squad</t>
+  </si>
+  <si>
+    <t>CSA_Destroyer_Droid_Company</t>
+  </si>
+  <si>
+    <t>X10_Group</t>
+  </si>
+  <si>
+    <t>Class_I_Company</t>
+  </si>
+  <si>
+    <t>Espo_Walker_Squad</t>
+  </si>
+  <si>
+    <t>GX12_Company</t>
+  </si>
+  <si>
+    <t>SX20_Company</t>
+  </si>
+  <si>
+    <t>Hailfire_Company</t>
+  </si>
+  <si>
+    <t>Persuader_Company</t>
+  </si>
+  <si>
+    <t>JX40_Group</t>
+  </si>
+  <si>
+    <t>Strikebreaker_Group</t>
+  </si>
+  <si>
+    <t>K222_Group</t>
+  </si>
+  <si>
+    <t>HRG_Commando_Squad</t>
+  </si>
+  <si>
+    <t>Hapan_Infantry_Squad</t>
+  </si>
+  <si>
+    <t>Maluri_Infantry_Squad</t>
+  </si>
+  <si>
+    <t>Requud_Infantry_Squad</t>
+  </si>
+  <si>
+    <t>Galney_Infantry_Squad</t>
+  </si>
+  <si>
+    <t>Hapan_LightTank_Company</t>
+  </si>
+  <si>
+    <t>Hapan_Artillery_Company</t>
+  </si>
+  <si>
+    <t>Hapan_Transport_Company</t>
+  </si>
+  <si>
+    <t>Hapan_Silanus_Company</t>
+  </si>
+  <si>
+    <t>Hapan_HeavyTank_Company</t>
+  </si>
+  <si>
+    <t>Hapan_Gunboat_Company</t>
+  </si>
+  <si>
+    <t>SsiRuuk_Squad</t>
+  </si>
+  <si>
+    <t>Yevetha_Infantry_Squad</t>
+  </si>
+  <si>
+    <t>Yevethan_Plex_Squad</t>
+  </si>
+  <si>
+    <t>Talon_Cloud_Car_Group</t>
   </si>
 </sst>
 </file>
@@ -1965,10 +2586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2C3333-FDB8-45E7-97B2-56CE751A9056}">
-  <dimension ref="A1:C275"/>
+  <dimension ref="A1:C482"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
+      <selection activeCell="A480" sqref="A480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5003,9 +5624,1044 @@
         <v>1</v>
       </c>
     </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>732</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1066">
-    <sortCondition ref="A1:A1066"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1008">
+    <sortCondition ref="A1:A1008"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated spreadsheet from CSV, added force generators to validation
</commit_message>
<xml_diff>
--- a/ReferenceSheet.xlsx
+++ b/ReferenceSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Phoenix Rising Work\EaWXStartingForces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75250B17-4DC9-4806-A016-DEC9FB46E573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF641BD-6A13-4398-855A-EA842363F70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C98BEB51-DB04-4536-A48A-2E267BCF39ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="748">
   <si>
     <t>Name</t>
   </si>
@@ -2235,6 +2235,51 @@
   </si>
   <si>
     <t>Talon_Cloud_Car_Group</t>
+  </si>
+  <si>
+    <t>Generate_Force_Rebel</t>
+  </si>
+  <si>
+    <t>Generate_Force_Empire</t>
+  </si>
+  <si>
+    <t>Generate_Force_Underworld</t>
+  </si>
+  <si>
+    <t>Generate_Force_Hutts</t>
+  </si>
+  <si>
+    <t>Generate_Force_EmpireoftheHand</t>
+  </si>
+  <si>
+    <t>Generate_Force_Pentastar</t>
+  </si>
+  <si>
+    <t>Generate_Force_Pirates</t>
+  </si>
+  <si>
+    <t>Generate_Force_Teradoc</t>
+  </si>
+  <si>
+    <t>Generate_Force_Hutt_Cartels</t>
+  </si>
+  <si>
+    <t>Generate_Force_Chiss</t>
+  </si>
+  <si>
+    <t>Generate_Force_Corellia</t>
+  </si>
+  <si>
+    <t>Generate_Force_SsiRuuvi_Imperium</t>
+  </si>
+  <si>
+    <t>Generate_Force_Hapes_Consortium</t>
+  </si>
+  <si>
+    <t>Generate_Force_Corporate_Sector</t>
+  </si>
+  <si>
+    <t>Generate_Force_Warlords</t>
   </si>
 </sst>
 </file>
@@ -2588,8 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2C3333-FDB8-45E7-97B2-56CE751A9056}">
   <dimension ref="A1:C482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
-      <selection activeCell="A480" sqref="A480"/>
+    <sheetView tabSelected="1" topLeftCell="A465" workbookViewId="0">
+      <selection activeCell="A487" sqref="A487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6669,10 +6714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36110936-ED2F-4F0C-A705-7877F81B8957}">
-  <dimension ref="A1:B250"/>
+  <dimension ref="A1:B265"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8680,6 +8725,81 @@
         <v>1</v>
       </c>
     </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>747</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>